<commit_message>
Commit to add the file: ContactUs.java
</commit_message>
<xml_diff>
--- a/target/test-classes/com/finexus/testDataProvider/TestCasesData.xlsx
+++ b/target/test-classes/com/finexus/testDataProvider/TestCasesData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>userName</t>
   </si>
@@ -66,19 +66,13 @@
   </si>
   <si>
     <t>blubd.softtech@gmail.com</t>
-  </si>
-  <si>
-    <t>wrongId@wrong.com</t>
-  </si>
-  <si>
-    <t>everlast#123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -126,12 +120,6 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -244,7 +232,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -273,8 +261,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -592,10 +578,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -627,37 +613,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>